<commit_message>
add short scale name to dict
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linh\Dropbox\Research\Projects\2020 SIBS 8282\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linh\Dropbox\Research\Projects\2020 SIBS 8282\8282-sibs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136A7427-A879-4A66-AAC9-96B558084D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7074B007-9382-498A-9643-3C446BB313F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="3105" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sibling relationship" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="168">
   <si>
     <t>variable</t>
   </si>
@@ -34,9 +34,6 @@
     <t>scale</t>
   </si>
   <si>
-    <t>subscale</t>
-  </si>
-  <si>
     <t>keying</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>How much do you show this sibling how to do things he or she doesn't know how to do?</t>
   </si>
   <si>
-    <t>Nurturance of sibling</t>
-  </si>
-  <si>
     <t>Q4</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>How much do you tell this sibling what to do?</t>
   </si>
   <si>
-    <t>Dominance of sibling</t>
-  </si>
-  <si>
     <t>Q6</t>
   </si>
   <si>
@@ -241,9 +232,6 @@
     <t>How much do you admire and respect this sibling?</t>
   </si>
   <si>
-    <t>Admiration of sibling</t>
-  </si>
-  <si>
     <t>Q15</t>
   </si>
   <si>
@@ -497,6 +485,45 @@
   </si>
   <si>
     <t>Date of survey completion</t>
+  </si>
+  <si>
+    <t>scale_short</t>
+  </si>
+  <si>
+    <t>S_YNURE</t>
+  </si>
+  <si>
+    <t>S_ENURY</t>
+  </si>
+  <si>
+    <t>S_YDOME</t>
+  </si>
+  <si>
+    <t>S_EDOMY</t>
+  </si>
+  <si>
+    <t>S_YADME</t>
+  </si>
+  <si>
+    <t>S_EADMY</t>
+  </si>
+  <si>
+    <t>Nurturance of sibling (self)</t>
+  </si>
+  <si>
+    <t>Nurturance of sibling (other)</t>
+  </si>
+  <si>
+    <t>Dominance of sibling (self)</t>
+  </si>
+  <si>
+    <t>Dominance of sibling (other)</t>
+  </si>
+  <si>
+    <t>Admiration of sibling (self)</t>
+  </si>
+  <si>
+    <t>Admiration of sibling (other)</t>
   </si>
 </sst>
 </file>
@@ -1340,9 +1367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,6 +1377,7 @@
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1366,1143 +1394,1269 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
         <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
         <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
       <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
         <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
         <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
       <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
         <v>40</v>
       </c>
-      <c r="D16" t="s">
-        <v>41</v>
+      <c r="E16" t="s">
+        <v>132</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>162</v>
+      </c>
+      <c r="E17" t="s">
+        <v>156</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>163</v>
+      </c>
+      <c r="E18" t="s">
+        <v>157</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>164</v>
+      </c>
+      <c r="E19" t="s">
+        <v>158</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>165</v>
+      </c>
+      <c r="E20" t="s">
+        <v>159</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>134</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>135</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="E24" t="s">
+        <v>136</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>137</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="E26" t="s">
+        <v>138</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>166</v>
+      </c>
+      <c r="E27" t="s">
+        <v>160</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>167</v>
+      </c>
+      <c r="E28" t="s">
+        <v>161</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="E29" t="s">
+        <v>139</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
         <v>40</v>
       </c>
-      <c r="D30" t="s">
-        <v>41</v>
+      <c r="E30" t="s">
+        <v>132</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>162</v>
+      </c>
+      <c r="E31" t="s">
+        <v>156</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>163</v>
+      </c>
+      <c r="E32" t="s">
+        <v>157</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>164</v>
+      </c>
+      <c r="E33" t="s">
+        <v>158</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>165</v>
+      </c>
+      <c r="E34" t="s">
+        <v>159</v>
       </c>
       <c r="F34">
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>133</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="E36" t="s">
+        <v>134</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
+        <v>135</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="E38" t="s">
+        <v>136</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
       <c r="G38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="E39" t="s">
+        <v>137</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="E40" t="s">
+        <v>138</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>166</v>
+      </c>
+      <c r="E41" t="s">
+        <v>160</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>167</v>
+      </c>
+      <c r="E42" t="s">
+        <v>161</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="E43" t="s">
+        <v>139</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" t="s">
         <v>40</v>
       </c>
-      <c r="D44" t="s">
-        <v>41</v>
+      <c r="E44" t="s">
+        <v>132</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D45" t="s">
-        <v>45</v>
+        <v>162</v>
+      </c>
+      <c r="E45" t="s">
+        <v>156</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
       <c r="G45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D46" t="s">
-        <v>45</v>
+        <v>163</v>
+      </c>
+      <c r="E46" t="s">
+        <v>157</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D47" t="s">
-        <v>50</v>
+        <v>164</v>
+      </c>
+      <c r="E47" t="s">
+        <v>158</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>165</v>
+      </c>
+      <c r="E48" t="s">
+        <v>159</v>
       </c>
       <c r="F48">
         <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D49" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="E49" t="s">
+        <v>133</v>
       </c>
       <c r="F49">
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="E50" t="s">
+        <v>134</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
+        <v>135</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="E52" t="s">
+        <v>136</v>
       </c>
       <c r="F52">
         <v>1</v>
       </c>
       <c r="G52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D53" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="E53" t="s">
+        <v>137</v>
       </c>
       <c r="F53">
         <v>1</v>
       </c>
       <c r="G53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D54" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="E54" t="s">
+        <v>138</v>
       </c>
       <c r="F54">
         <v>1</v>
       </c>
       <c r="G54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>166</v>
+      </c>
+      <c r="E55" t="s">
+        <v>160</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B56" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>167</v>
+      </c>
+      <c r="E56" t="s">
+        <v>161</v>
       </c>
       <c r="F56">
         <v>1</v>
       </c>
       <c r="G56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B57" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D57" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="E57" t="s">
+        <v>139</v>
       </c>
       <c r="F57">
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>